<commit_message>
Validator Constraints issues, add the non-working input file and ARMA
</commit_message>
<xml_diff>
--- a/tests/integration_tests/ARMA/Sine_1/Data_1_save_function.xlsx
+++ b/tests/integration_tests/ARMA/Sine_1/Data_1_save_function.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\wanghy_fork\HERON\tests\integration_tests\ARMA\Sine_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38C175D-79AC-4B00-9455-F29A87C8B77C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996DD55B-FB31-4392-A6B5-CDC95A12A98E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23340" yWindow="3780" windowWidth="12420" windowHeight="14145" activeTab="2" xr2:uid="{D61530F6-2741-4636-AC6C-BF1700677F29}"/>
+    <workbookView xWindow="17625" yWindow="3120" windowWidth="12420" windowHeight="14145" activeTab="1" xr2:uid="{D61530F6-2741-4636-AC6C-BF1700677F29}"/>
   </bookViews>
   <sheets>
     <sheet name="How many to Charge" sheetId="1" r:id="rId1"/>
@@ -90,12 +90,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,10 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691BF2F7-8E89-4F17-A271-B4DAE608451B}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,7 +1062,7 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <f>C$1*SIN(PI()/12*B4)+C$2</f>
         <v>-1147.5</v>
       </c>
@@ -1076,7 +1090,7 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <f t="shared" ref="C5:C27" si="0">C$1*SIN(PI()/12*B5)+C$2</f>
         <v>-1128.0885716173109</v>
       </c>
@@ -1104,7 +1118,7 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <f t="shared" si="0"/>
         <v>-1110</v>
       </c>
@@ -1132,7 +1146,7 @@
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <f t="shared" si="0"/>
         <v>-1094.4669914110088</v>
       </c>
@@ -1160,7 +1174,7 @@
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <f t="shared" si="0"/>
         <v>-1082.548094716167</v>
       </c>
@@ -1188,7 +1202,7 @@
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <f t="shared" si="0"/>
         <v>-1075.05556302832</v>
       </c>
@@ -1216,7 +1230,7 @@
       <c r="B10">
         <v>6</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <f t="shared" si="0"/>
         <v>-1072.5</v>
       </c>
@@ -1244,7 +1258,7 @@
       <c r="B11">
         <v>7</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <f t="shared" si="0"/>
         <v>-1075.05556302832</v>
       </c>
@@ -1272,7 +1286,7 @@
       <c r="B12">
         <v>8</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <f t="shared" si="0"/>
         <v>-1082.548094716167</v>
       </c>
@@ -1300,7 +1314,7 @@
       <c r="B13">
         <v>9</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <f t="shared" si="0"/>
         <v>-1094.4669914110088</v>
       </c>
@@ -1328,7 +1342,7 @@
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <f t="shared" si="0"/>
         <v>-1110</v>
       </c>
@@ -1356,7 +1370,7 @@
       <c r="B15">
         <v>11</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <f t="shared" si="0"/>
         <v>-1128.0885716173109</v>
       </c>
@@ -1384,7 +1398,7 @@
       <c r="B16">
         <v>12</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="4">
         <f t="shared" si="0"/>
         <v>-1147.5</v>
       </c>
@@ -1412,7 +1426,7 @@
       <c r="B17">
         <v>13</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <f t="shared" si="0"/>
         <v>-1166.9114283826891</v>
       </c>
@@ -1440,7 +1454,7 @@
       <c r="B18">
         <v>14</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="4">
         <f t="shared" si="0"/>
         <v>-1185</v>
       </c>
@@ -1468,7 +1482,7 @@
       <c r="B19">
         <v>15</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="4">
         <f t="shared" si="0"/>
         <v>-1200.5330085889909</v>
       </c>
@@ -1496,7 +1510,7 @@
       <c r="B20">
         <v>16</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="4">
         <f t="shared" si="0"/>
         <v>-1212.451905283833</v>
       </c>
@@ -1524,7 +1538,7 @@
       <c r="B21">
         <v>17</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="4">
         <f t="shared" si="0"/>
         <v>-1219.94443697168</v>
       </c>
@@ -1552,7 +1566,7 @@
       <c r="B22">
         <v>18</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="4">
         <f t="shared" si="0"/>
         <v>-1222.5</v>
       </c>
@@ -1580,7 +1594,7 @@
       <c r="B23">
         <v>19</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="4">
         <f t="shared" si="0"/>
         <v>-1219.94443697168</v>
       </c>
@@ -1608,7 +1622,7 @@
       <c r="B24">
         <v>20</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="4">
         <f t="shared" si="0"/>
         <v>-1212.451905283833</v>
       </c>
@@ -1636,7 +1650,7 @@
       <c r="B25">
         <v>21</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="4">
         <f t="shared" si="0"/>
         <v>-1200.5330085889912</v>
       </c>
@@ -1664,7 +1678,7 @@
       <c r="B26">
         <v>22</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="4">
         <f t="shared" si="0"/>
         <v>-1185</v>
       </c>
@@ -1692,7 +1706,7 @@
       <c r="B27">
         <v>23</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="4">
         <f t="shared" si="0"/>
         <v>-1166.9114283826891</v>
       </c>
@@ -1740,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D53159-4083-44D9-B67B-9D1E4CA1C7F1}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C27"/>
     </sheetView>
   </sheetViews>
@@ -1797,7 +1811,7 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <f>C$1*SIN(PI()/12*B4)+C$2</f>
         <v>-1145</v>
       </c>
@@ -1825,7 +1839,7 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <f t="shared" ref="C5:C27" si="0">C$1*SIN(PI()/12*B5)+C$2</f>
         <v>-1125.5885716173109</v>
       </c>
@@ -1853,7 +1867,7 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <f t="shared" si="0"/>
         <v>-1107.5</v>
       </c>
@@ -1881,7 +1895,7 @@
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>-1091.9669914110088</v>
       </c>
@@ -1909,7 +1923,7 @@
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <f t="shared" si="0"/>
         <v>-1080.048094716167</v>
       </c>
@@ -1937,7 +1951,7 @@
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <f t="shared" si="0"/>
         <v>-1072.55556302832</v>
       </c>
@@ -1965,7 +1979,7 @@
       <c r="B10">
         <v>6</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <f t="shared" si="0"/>
         <v>-1070</v>
       </c>
@@ -1993,7 +2007,7 @@
       <c r="B11">
         <v>7</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <f t="shared" si="0"/>
         <v>-1072.55556302832</v>
       </c>
@@ -2021,7 +2035,7 @@
       <c r="B12">
         <v>8</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <f t="shared" si="0"/>
         <v>-1080.048094716167</v>
       </c>
@@ -2049,7 +2063,7 @@
       <c r="B13">
         <v>9</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <f t="shared" si="0"/>
         <v>-1091.9669914110088</v>
       </c>
@@ -2077,7 +2091,7 @@
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <f t="shared" si="0"/>
         <v>-1107.5</v>
       </c>
@@ -2105,7 +2119,7 @@
       <c r="B15">
         <v>11</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="3">
         <f t="shared" si="0"/>
         <v>-1125.5885716173109</v>
       </c>
@@ -2133,7 +2147,7 @@
       <c r="B16">
         <v>12</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <f t="shared" si="0"/>
         <v>-1145</v>
       </c>
@@ -2161,7 +2175,7 @@
       <c r="B17">
         <v>13</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <f t="shared" si="0"/>
         <v>-1164.4114283826891</v>
       </c>
@@ -2189,7 +2203,7 @@
       <c r="B18">
         <v>14</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="3">
         <f t="shared" si="0"/>
         <v>-1182.5</v>
       </c>
@@ -2217,7 +2231,7 @@
       <c r="B19">
         <v>15</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="3">
         <f t="shared" si="0"/>
         <v>-1198.0330085889909</v>
       </c>
@@ -2245,7 +2259,7 @@
       <c r="B20">
         <v>16</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="3">
         <f t="shared" si="0"/>
         <v>-1209.951905283833</v>
       </c>
@@ -2273,7 +2287,7 @@
       <c r="B21">
         <v>17</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="3">
         <f t="shared" si="0"/>
         <v>-1217.44443697168</v>
       </c>
@@ -2301,7 +2315,7 @@
       <c r="B22">
         <v>18</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="3">
         <f t="shared" si="0"/>
         <v>-1220</v>
       </c>
@@ -2329,7 +2343,7 @@
       <c r="B23">
         <v>19</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="3">
         <f t="shared" si="0"/>
         <v>-1217.44443697168</v>
       </c>
@@ -2357,7 +2371,7 @@
       <c r="B24">
         <v>20</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="3">
         <f t="shared" si="0"/>
         <v>-1209.951905283833</v>
       </c>
@@ -2385,7 +2399,7 @@
       <c r="B25">
         <v>21</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="3">
         <f t="shared" si="0"/>
         <v>-1198.0330085889912</v>
       </c>
@@ -2413,7 +2427,7 @@
       <c r="B26">
         <v>22</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="3">
         <f t="shared" si="0"/>
         <v>-1182.5</v>
       </c>
@@ -2441,7 +2455,7 @@
       <c r="B27">
         <v>23</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="3">
         <f t="shared" si="0"/>
         <v>-1164.4114283826891</v>
       </c>

</xml_diff>

<commit_message>
sine week arma issue
</commit_message>
<xml_diff>
--- a/tests/integration_tests/ARMA/Sine_1/Data_1_save_function.xlsx
+++ b/tests/integration_tests/ARMA/Sine_1/Data_1_save_function.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\wanghy_fork\HERON\tests\integration_tests\ARMA\Sine_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996DD55B-FB31-4392-A6B5-CDC95A12A98E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88A99C1-DB63-497D-A50C-3570F070242C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17625" yWindow="3120" windowWidth="12420" windowHeight="14145" activeTab="1" xr2:uid="{D61530F6-2741-4636-AC6C-BF1700677F29}"/>
+    <workbookView xWindow="19605" yWindow="1455" windowWidth="17265" windowHeight="17130" activeTab="2" xr2:uid="{D61530F6-2741-4636-AC6C-BF1700677F29}"/>
   </bookViews>
   <sheets>
     <sheet name="How many to Charge" sheetId="1" r:id="rId1"/>
@@ -1022,7 +1022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691BF2F7-8E89-4F17-A271-B4DAE608451B}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1754,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D53159-4083-44D9-B67B-9D1E4CA1C7F1}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:C27"/>
     </sheetView>
   </sheetViews>
@@ -1770,7 +1770,7 @@
         <v>6</v>
       </c>
       <c r="C1">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1778,7 +1778,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>-1145</v>
+        <v>-1143</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1813,23 +1813,23 @@
       </c>
       <c r="C4" s="3">
         <f>C$1*SIN(PI()/12*B4)+C$2</f>
-        <v>-1145</v>
+        <v>-1143</v>
       </c>
       <c r="D4" s="2">
         <f>(-1180.838-C4)</f>
-        <v>-35.837999999999965</v>
+        <v>-37.837999999999965</v>
       </c>
       <c r="E4" s="2">
         <f>SUM(D$4:D4)</f>
-        <v>-35.837999999999965</v>
+        <v>-37.837999999999965</v>
       </c>
       <c r="F4" s="2">
         <f>C$1*SIN(PI()/12*B4)+C$2</f>
-        <v>-1145</v>
+        <v>-1143</v>
       </c>
       <c r="G4" s="2">
         <f>C$1*SIN(PI()/12*B4)+C$2</f>
-        <v>-1145</v>
+        <v>-1143</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1841,23 +1841,23 @@
       </c>
       <c r="C5" s="3">
         <f t="shared" ref="C5:C27" si="0">C$1*SIN(PI()/12*B5)+C$2</f>
-        <v>-1125.5885716173109</v>
+        <v>-1122.2944763917983</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ref="D5:D27" si="1">(-1180.838-C5)</f>
-        <v>-55.249428382689075</v>
+        <v>-58.543523608201667</v>
       </c>
       <c r="E5" s="2">
         <f>SUM(D$4:D5)</f>
-        <v>-91.087428382689041</v>
+        <v>-96.381523608201633</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" ref="F5:F27" si="2">C$1*SIN(PI()/12*B5)+C$2</f>
-        <v>-1125.5885716173109</v>
+        <v>-1122.2944763917983</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" ref="G5:G27" si="3">C$1*SIN(PI()/12*B5)+C$2</f>
-        <v>-1125.5885716173109</v>
+        <v>-1122.2944763917983</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1869,23 +1869,23 @@
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>-1107.5</v>
+        <v>-1103</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="1"/>
-        <v>-73.337999999999965</v>
+        <v>-77.837999999999965</v>
       </c>
       <c r="E6" s="2">
         <f>SUM(D$4:D6)</f>
-        <v>-164.42542838268901</v>
+        <v>-174.2195236082016</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="2"/>
-        <v>-1107.5</v>
+        <v>-1103</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="3"/>
-        <v>-1107.5</v>
+        <v>-1103</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1897,23 +1897,23 @@
       </c>
       <c r="C7" s="3">
         <f t="shared" si="0"/>
-        <v>-1091.9669914110088</v>
+        <v>-1086.4314575050762</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="1"/>
-        <v>-88.871008588991117</v>
+        <v>-94.406542494923769</v>
       </c>
       <c r="E7" s="2">
         <f>SUM(D$4:D7)</f>
-        <v>-253.29643697168012</v>
+        <v>-268.62606610312537</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="2"/>
-        <v>-1091.9669914110088</v>
+        <v>-1086.4314575050762</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="3"/>
-        <v>-1091.9669914110088</v>
+        <v>-1086.4314575050762</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1925,23 +1925,23 @@
       </c>
       <c r="C8" s="3">
         <f t="shared" si="0"/>
-        <v>-1080.048094716167</v>
+        <v>-1073.7179676972448</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="1"/>
-        <v>-100.78990528383292</v>
+        <v>-107.12003230275513</v>
       </c>
       <c r="E8" s="2">
         <f>SUM(D$4:D8)</f>
-        <v>-354.08634225551305</v>
+        <v>-375.7460984058805</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="2"/>
-        <v>-1080.048094716167</v>
+        <v>-1073.7179676972448</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="3"/>
-        <v>-1080.048094716167</v>
+        <v>-1073.7179676972448</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1953,23 +1953,23 @@
       </c>
       <c r="C9" s="3">
         <f t="shared" si="0"/>
-        <v>-1072.55556302832</v>
+        <v>-1065.7259338968745</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>-108.28243697168</v>
+        <v>-115.11206610312547</v>
       </c>
       <c r="E9" s="2">
         <f>SUM(D$4:D9)</f>
-        <v>-462.36877922719304</v>
+        <v>-490.85816450900597</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="2"/>
-        <v>-1072.55556302832</v>
+        <v>-1065.7259338968745</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="3"/>
-        <v>-1072.55556302832</v>
+        <v>-1065.7259338968745</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1981,23 +1981,23 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" si="0"/>
-        <v>-1070</v>
+        <v>-1063</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>-110.83799999999997</v>
+        <v>-117.83799999999997</v>
       </c>
       <c r="E10" s="2">
         <f>SUM(D$4:D10)</f>
-        <v>-573.20677922719301</v>
+        <v>-608.69616450900594</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="2"/>
-        <v>-1070</v>
+        <v>-1063</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="3"/>
-        <v>-1070</v>
+        <v>-1063</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2009,23 +2009,23 @@
       </c>
       <c r="C11" s="3">
         <f t="shared" si="0"/>
-        <v>-1072.55556302832</v>
+        <v>-1065.7259338968745</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>-108.28243697168</v>
+        <v>-115.11206610312547</v>
       </c>
       <c r="E11" s="2">
         <f>SUM(D$4:D11)</f>
-        <v>-681.48921619887301</v>
+        <v>-723.80823061213141</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="2"/>
-        <v>-1072.55556302832</v>
+        <v>-1065.7259338968745</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="3"/>
-        <v>-1072.55556302832</v>
+        <v>-1065.7259338968745</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2037,23 +2037,23 @@
       </c>
       <c r="C12" s="3">
         <f t="shared" si="0"/>
-        <v>-1080.048094716167</v>
+        <v>-1073.7179676972448</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>-100.78990528383292</v>
+        <v>-107.12003230275513</v>
       </c>
       <c r="E12" s="2">
         <f>SUM(D$4:D12)</f>
-        <v>-782.27912148270593</v>
+        <v>-830.92826291488655</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="2"/>
-        <v>-1080.048094716167</v>
+        <v>-1073.7179676972448</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="3"/>
-        <v>-1080.048094716167</v>
+        <v>-1073.7179676972448</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2065,23 +2065,23 @@
       </c>
       <c r="C13" s="3">
         <f t="shared" si="0"/>
-        <v>-1091.9669914110088</v>
+        <v>-1086.4314575050762</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>-88.871008588991117</v>
+        <v>-94.406542494923769</v>
       </c>
       <c r="E13" s="2">
         <f>SUM(D$4:D13)</f>
-        <v>-871.15013007169705</v>
+        <v>-925.33480540981031</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="2"/>
-        <v>-1091.9669914110088</v>
+        <v>-1086.4314575050762</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="3"/>
-        <v>-1091.9669914110088</v>
+        <v>-1086.4314575050762</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2093,23 +2093,23 @@
       </c>
       <c r="C14" s="3">
         <f t="shared" si="0"/>
-        <v>-1107.5</v>
+        <v>-1103</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
-        <v>-73.337999999999965</v>
+        <v>-77.837999999999965</v>
       </c>
       <c r="E14" s="2">
         <f>SUM(D$4:D14)</f>
-        <v>-944.48813007169701</v>
+        <v>-1003.1728054098103</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="2"/>
-        <v>-1107.5</v>
+        <v>-1103</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="3"/>
-        <v>-1107.5</v>
+        <v>-1103</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2121,23 +2121,23 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" si="0"/>
-        <v>-1125.5885716173109</v>
+        <v>-1122.2944763917983</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="1"/>
-        <v>-55.249428382689075</v>
+        <v>-58.543523608201667</v>
       </c>
       <c r="E15" s="2">
         <f>SUM(D$4:D15)</f>
-        <v>-999.73755845438609</v>
+        <v>-1061.7163290180119</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="2"/>
-        <v>-1125.5885716173109</v>
+        <v>-1122.2944763917983</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="3"/>
-        <v>-1125.5885716173109</v>
+        <v>-1122.2944763917983</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2149,23 +2149,23 @@
       </c>
       <c r="C16" s="3">
         <f t="shared" si="0"/>
-        <v>-1145</v>
+        <v>-1143</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>-35.837999999999965</v>
+        <v>-37.837999999999965</v>
       </c>
       <c r="E16" s="2">
         <f>SUM(D$4:D16)</f>
-        <v>-1035.5755584543861</v>
+        <v>-1099.5543290180119</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="2"/>
-        <v>-1145</v>
+        <v>-1143</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="3"/>
-        <v>-1145</v>
+        <v>-1143</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2177,23 +2177,23 @@
       </c>
       <c r="C17" s="3">
         <f t="shared" si="0"/>
-        <v>-1164.4114283826891</v>
+        <v>-1163.7055236082017</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>-16.426571617310856</v>
+        <v>-17.132476391798264</v>
       </c>
       <c r="E17" s="2">
         <f>SUM(D$4:D17)</f>
-        <v>-1052.0021300716969</v>
+        <v>-1116.6868054098102</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="2"/>
-        <v>-1164.4114283826891</v>
+        <v>-1163.7055236082017</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="3"/>
-        <v>-1164.4114283826891</v>
+        <v>-1163.7055236082017</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2205,23 +2205,23 @@
       </c>
       <c r="C18" s="3">
         <f t="shared" si="0"/>
-        <v>-1182.5</v>
+        <v>-1183</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>1.6620000000000346</v>
+        <v>2.1620000000000346</v>
       </c>
       <c r="E18" s="2">
         <f>SUM(D$4:D18)</f>
-        <v>-1050.3401300716969</v>
+        <v>-1114.5248054098101</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="2"/>
-        <v>-1182.5</v>
+        <v>-1183</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="3"/>
-        <v>-1182.5</v>
+        <v>-1183</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2233,23 +2233,23 @@
       </c>
       <c r="C19" s="3">
         <f t="shared" si="0"/>
-        <v>-1198.0330085889909</v>
+        <v>-1199.5685424949238</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
-        <v>17.195008588990959</v>
+        <v>18.730542494923839</v>
       </c>
       <c r="E19" s="2">
         <f>SUM(D$4:D19)</f>
-        <v>-1033.1451214827059</v>
+        <v>-1095.7942629148863</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="2"/>
-        <v>-1198.0330085889909</v>
+        <v>-1199.5685424949238</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="3"/>
-        <v>-1198.0330085889909</v>
+        <v>-1199.5685424949238</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2261,23 +2261,23 @@
       </c>
       <c r="C20" s="3">
         <f t="shared" si="0"/>
-        <v>-1209.951905283833</v>
+        <v>-1212.2820323027552</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="1"/>
-        <v>29.113905283832992</v>
+        <v>31.444032302755204</v>
       </c>
       <c r="E20" s="2">
         <f>SUM(D$4:D20)</f>
-        <v>-1004.0312161988729</v>
+        <v>-1064.3502306121311</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="2"/>
-        <v>-1209.951905283833</v>
+        <v>-1212.2820323027552</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="3"/>
-        <v>-1209.951905283833</v>
+        <v>-1212.2820323027552</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2289,23 +2289,23 @@
       </c>
       <c r="C21" s="3">
         <f t="shared" si="0"/>
-        <v>-1217.44443697168</v>
+        <v>-1220.2740661031255</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="1"/>
-        <v>36.606436971680068</v>
+        <v>39.43606610312554</v>
       </c>
       <c r="E21" s="2">
         <f>SUM(D$4:D21)</f>
-        <v>-967.42477922719286</v>
+        <v>-1024.9141645090056</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="2"/>
-        <v>-1217.44443697168</v>
+        <v>-1220.2740661031255</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="3"/>
-        <v>-1217.44443697168</v>
+        <v>-1220.2740661031255</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2317,23 +2317,23 @@
       </c>
       <c r="C22" s="3">
         <f t="shared" si="0"/>
-        <v>-1220</v>
+        <v>-1223</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="1"/>
-        <v>39.162000000000035</v>
+        <v>42.162000000000035</v>
       </c>
       <c r="E22" s="2">
         <f>SUM(D$4:D22)</f>
-        <v>-928.26277922719282</v>
+        <v>-982.75216450900552</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="2"/>
-        <v>-1220</v>
+        <v>-1223</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="3"/>
-        <v>-1220</v>
+        <v>-1223</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2345,23 +2345,23 @@
       </c>
       <c r="C23" s="3">
         <f t="shared" si="0"/>
-        <v>-1217.44443697168</v>
+        <v>-1220.2740661031255</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="1"/>
-        <v>36.606436971680068</v>
+        <v>39.43606610312554</v>
       </c>
       <c r="E23" s="2">
         <f>SUM(D$4:D23)</f>
-        <v>-891.65634225551275</v>
+        <v>-943.31609840587998</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="2"/>
-        <v>-1217.44443697168</v>
+        <v>-1220.2740661031255</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="3"/>
-        <v>-1217.44443697168</v>
+        <v>-1220.2740661031255</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2373,23 +2373,23 @@
       </c>
       <c r="C24" s="3">
         <f t="shared" si="0"/>
-        <v>-1209.951905283833</v>
+        <v>-1212.2820323027552</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" si="1"/>
-        <v>29.113905283832992</v>
+        <v>31.444032302755204</v>
       </c>
       <c r="E24" s="2">
         <f>SUM(D$4:D24)</f>
-        <v>-862.54243697167976</v>
+        <v>-911.87206610312478</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="2"/>
-        <v>-1209.951905283833</v>
+        <v>-1212.2820323027552</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="3"/>
-        <v>-1209.951905283833</v>
+        <v>-1212.2820323027552</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2401,23 +2401,23 @@
       </c>
       <c r="C25" s="3">
         <f t="shared" si="0"/>
-        <v>-1198.0330085889912</v>
+        <v>-1199.5685424949238</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" si="1"/>
-        <v>17.195008588991186</v>
+        <v>18.730542494923839</v>
       </c>
       <c r="E25" s="2">
         <f>SUM(D$4:D25)</f>
-        <v>-845.34742838268858</v>
+        <v>-893.14152360820094</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="2"/>
-        <v>-1198.0330085889912</v>
+        <v>-1199.5685424949238</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" si="3"/>
-        <v>-1198.0330085889912</v>
+        <v>-1199.5685424949238</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2429,23 +2429,23 @@
       </c>
       <c r="C26" s="3">
         <f t="shared" si="0"/>
-        <v>-1182.5</v>
+        <v>-1183</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="1"/>
-        <v>1.6620000000000346</v>
+        <v>2.1620000000000346</v>
       </c>
       <c r="E26" s="2">
         <f>SUM(D$4:D26)</f>
-        <v>-843.68542838268854</v>
+        <v>-890.97952360820091</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="2"/>
-        <v>-1182.5</v>
+        <v>-1183</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" si="3"/>
-        <v>-1182.5</v>
+        <v>-1183</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2457,23 +2457,23 @@
       </c>
       <c r="C27" s="3">
         <f t="shared" si="0"/>
-        <v>-1164.4114283826891</v>
+        <v>-1163.7055236082017</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="1"/>
-        <v>-16.426571617310856</v>
+        <v>-17.132476391798264</v>
       </c>
       <c r="E27" s="2">
         <f>SUM(D$4:D27)</f>
-        <v>-860.1119999999994</v>
+        <v>-908.11199999999917</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" si="2"/>
-        <v>-1164.4114283826891</v>
+        <v>-1163.7055236082017</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" si="3"/>
-        <v>-1164.4114283826891</v>
+        <v>-1163.7055236082017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>